<commit_message>
add rotation in daca
</commit_message>
<xml_diff>
--- a/Data/DrillingReplayFileModel.xlsx
+++ b/Data/DrillingReplayFileModel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linje\EPITA\Res\DrillDigitalTwin\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didcoa000328\Documents\DrillDigitalTwin\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A144FBD-C1B7-4C40-8DCE-F6627B42132B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C9CA77-D0BC-4B31-A537-2CEFBE00DAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{222BA2F0-3CB0-4FCA-BB74-0876CD06BA44}"/>
+    <workbookView xWindow="12870" yWindow="-16395" windowWidth="29040" windowHeight="15720" xr2:uid="{222BA2F0-3CB0-4FCA-BB74-0876CD06BA44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>RT_Temp</t>
+  </si>
+  <si>
+    <t>DrillBit_Rotation</t>
   </si>
 </sst>
 </file>
@@ -446,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE3BADA-EA87-4016-B341-A1419F13AEF6}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,21 +480,24 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add layer in data csv
</commit_message>
<xml_diff>
--- a/Data/DrillingReplayFileModel.xlsx
+++ b/Data/DrillingReplayFileModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didcoa000328\Documents\DrillDigitalTwin\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C9CA77-D0BC-4B31-A537-2CEFBE00DAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA86E717-8322-4971-9989-EF32F3C5E384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="-16395" windowWidth="29040" windowHeight="15720" xr2:uid="{222BA2F0-3CB0-4FCA-BB74-0876CD06BA44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{222BA2F0-3CB0-4FCA-BB74-0876CD06BA44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>DrillBit_Rotation</t>
+  </si>
+  <si>
+    <t>DB_Torque</t>
+  </si>
+  <si>
+    <t>Layer</t>
   </si>
 </sst>
 </file>
@@ -449,15 +455,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE3BADA-EA87-4016-B341-A1419F13AEF6}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,6 +505,12 @@
       </c>
       <c r="N1" t="s">
         <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>